<commit_message>
rimozione tm da codice produttore
</commit_message>
<xml_diff>
--- a/input/sconti.xlsx
+++ b/input/sconti.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a1/PycharmProjects/IMPORT BELTRAMI/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F84DF1B-A224-BA42-A39F-CD7D18FD85B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E490A9-0CD7-914D-A6F4-113C4E22620E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="38400" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
   <si>
     <t>FAMIGLIA</t>
   </si>
@@ -209,9 +209,6 @@
   </si>
   <si>
     <t>CORIMA</t>
-  </si>
-  <si>
-    <t>ZIP</t>
   </si>
   <si>
     <t>MUC</t>
@@ -618,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="G76" sqref="G76"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62:XFD62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2079,22 +2076,22 @@
       <c r="A64" t="s">
         <v>65</v>
       </c>
-      <c r="B64">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C64">
-        <v>1.05</v>
-      </c>
-      <c r="D64">
-        <v>1</v>
-      </c>
-      <c r="E64">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F64">
-        <v>1.05</v>
-      </c>
-      <c r="G64">
+      <c r="B64" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C64" s="2">
+        <v>1.05</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1</v>
+      </c>
+      <c r="E64" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F64" s="2">
+        <v>1.05</v>
+      </c>
+      <c r="G64" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2125,24 +2122,6 @@
       <c r="A66" t="s">
         <v>67</v>
       </c>
-      <c r="B66" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C66" s="2">
-        <v>1.05</v>
-      </c>
-      <c r="D66" s="2">
-        <v>1</v>
-      </c>
-      <c r="E66" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F66" s="2">
-        <v>1.05</v>
-      </c>
-      <c r="G66" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
@@ -2158,6 +2137,24 @@
       <c r="A69" t="s">
         <v>70</v>
       </c>
+      <c r="B69">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C69">
+        <v>1.05</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F69">
+        <v>1.05</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
@@ -2170,7 +2167,7 @@
         <v>1.05</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="E70">
         <v>1.1000000000000001</v>
@@ -2179,31 +2176,13 @@
         <v>1.05</v>
       </c>
       <c r="G70">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>72</v>
       </c>
-      <c r="B71">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C71">
-        <v>1.05</v>
-      </c>
-      <c r="D71">
-        <v>0.99</v>
-      </c>
-      <c r="E71">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F71">
-        <v>1.05</v>
-      </c>
-      <c r="G71">
-        <v>0.99</v>
-      </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
@@ -2213,11 +2192,6 @@
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>